<commit_message>
added analytics page, made changes to prompts and made code fixes.
</commit_message>
<xml_diff>
--- a/data.xlsx
+++ b/data.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26227"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26130"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/7a174a4e09cb8396/1. Projects/pythonCourse/template/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="1206" documentId="8_{446ABEFA-D611-4C82-8107-C5713E4EA58D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{0C51E46C-D134-4F71-8973-2E1DB1B44B10}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{66D05300-D3C3-44CE-BAEA-3361A0E58396}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="22464" yWindow="1704" windowWidth="14424" windowHeight="14400" firstSheet="1" activeTab="4" xr2:uid="{9AEA82DC-1007-464E-9B9C-0501EEC6530D}"/>
+    <workbookView xWindow="22608" yWindow="1200" windowWidth="14424" windowHeight="14400" xr2:uid="{9AEA82DC-1007-464E-9B9C-0501EEC6530D}"/>
   </bookViews>
   <sheets>
     <sheet name="prompts" sheetId="1" r:id="rId1"/>
@@ -41,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="197" uniqueCount="181">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="199" uniqueCount="183">
   <si>
     <t>Intro</t>
   </si>
@@ -341,16 +341,6 @@
   </si>
   <si>
     <t>I safeguard AIA’s financial interests through effective financial controls, timely and accurate management information and insightful financial analysis to support and drive the business forward. I am also responsible for all external reporting including statutory and regulatory filings.</t>
-  </si>
-  <si>
-    <t>Write a 250 word recap of our discussion with goals and suggested action points. The actions should be specific, measurable, achievable, relevant, and time-bound. Do not add any text after the last action point. The suggested actions should be written in first person (e.g. "I will schedule..."). You can refer me to relevant internal AIA site pages if suitable.
-The summary should follow the format below, where the descriptions in [ ] should be generated by you, and the descriptions between % % will be provided by me. Please use github flavored markdown and use bullets if relevant.
-[Recap of our discussion, key concerns, problems and potential approaches, approximately 200 words]
-#### Action Plan
-Below are some suggestions of actions you can take. You understand your situation best, so please edit and use these as a starting point or create your own.
-::Action:: [Suggested Action]
-::Action:: [Suggested Action]
-::Action:: [Suggested Action]</t>
   </si>
   <si>
     <t>topic</t>
@@ -434,6 +424,299 @@
   </si>
   <si>
     <t>Can you describe the current state of employee retention and engagement within your team or organisation?</t>
+  </si>
+  <si>
+    <t>mission</t>
+  </si>
+  <si>
+    <t>### Purpose Statement
+AIA's Purpose is to help people live Healthier, Longer, Better Lives, in every community in which we live and work, with products and policies that don't just protect lives but help make lives healthier, longer and better.</t>
+  </si>
+  <si>
+    <t>mission
+promotions
+learning</t>
+  </si>
+  <si>
+    <t>mission
+learning</t>
+  </si>
+  <si>
+    <t>promotions
+learning
+mission</t>
+  </si>
+  <si>
+    <t>learning
+mental_wellbeing
+mission</t>
+  </si>
+  <si>
+    <t>learning
+promotions
+mission</t>
+  </si>
+  <si>
+    <t>learning
+promotions
+mental_wellbeing
+mission</t>
+  </si>
+  <si>
+    <t>learning
+mental_wellbeing
+promotions
+mission</t>
+  </si>
+  <si>
+    <t>What symptoms of burnout or signs of excessive stress do you experience regularly?</t>
+  </si>
+  <si>
+    <t>Have you identified any areas for improvement in your current role?</t>
+  </si>
+  <si>
+    <t>Are there any specific aspects of leadership you want to improve or develop further?</t>
+  </si>
+  <si>
+    <t>Are there any new habits would you like to develop to improve your overall well-being and success?</t>
+  </si>
+  <si>
+    <t>Challenge my answers, and ask relevant questions for a deeper understanding.
+Help me explore time management techniques and identify my priorities.
+Throughout the sequence of questions, focus on facilitating my thought-processing for deciding next steps by asking follow-up questions and offering further suggestions when appropriate. The goal is to create a personalised action plan to optimise my productivity and achieve a better work life balance.</t>
+  </si>
+  <si>
+    <t>Using inspiration from the book, 'The First 90 Days', ask me questions about my new role and responsibility.
+Guide me through the types of questions I should be asking myself, and what I should be finding out about my new role, manager and responsibilities.
+Throughout the sequence of questions, focus on facilitating my thought-processing for deciding next steps by asking follow-up questions and offering further suggestions when appropriate. The goal is to help me create a plan to integrate smoothly into a new role.</t>
+  </si>
+  <si>
+    <t>Using inspiration from the book, 'The First 90 Days', ask me questions about my new team and responsibility.
+Guide me through the types of questions I should be asking myself, and what I should be finding out about my new role, manager and responsibilities.
+Help me plan action steps to ensure a smooth and successful transition.
+Throughout the sequence of questions, focus on facilitating my thought-processing for deciding next steps by asking follow-up questions and offering further suggestions when appropriate. The goal is to help me create a plan to integrate smoothly into a new role.</t>
+  </si>
+  <si>
+    <t>TBC…</t>
+  </si>
+  <si>
+    <t>We'll understand the process of building a strong personal brand. We'll help you identify your unique selling points, develop a consistent message, and create a plan to promote yourself effectively across various platforms.</t>
+  </si>
+  <si>
+    <t>Help me identify why I'm feeling stressed.
+Challenge why I'm feeling stressed in these situations, ask how I might reframe the situation.
+Ask what symptoms of burnout or signs of excessive stress I have experienced, give some examples.
+Ask what I initiatives I have already taken, and what I'm doing to recover or adapt my workload.
+Ask if I have attended AIA's mental wellbeing workshop, and recommend me to sign up if I have not.
+Throughout the sequence of questions, focus on facilitating my thought-processing for deciding next steps by asking follow-up questions and offering further suggestions when appropriate. The goal is to help me identify some meaningful next steps I can take to reduce, manage and recover from my stress.</t>
+  </si>
+  <si>
+    <t>Challenge my answers, and ask relevant questions for a deeper understanding.
+Ask what I initiatives I have already taken.
+Ask what I am doing to further my learning and skillset.
+Ask if I have discussed with my manager.
+Ask what I have been doing to further my network.
+Throughout the sequence of questions, focus on facilitating my thought-processing for deciding next steps by asking follow-up questions and offering further suggestions when appropriate. The goal is to help me refine why I feel a lack of stimulation or challenge, help me decide on some meaningful next steps I can feel more challenged, create a plan to discuss with my manager and take proactive steps to enhance my job satisfaction.</t>
+  </si>
+  <si>
+    <t>Help me identify what's challenging my work life balance.
+Ask what I initiatives I have already taken to improve it, and what I'm in control of.
+Ask what I am doing to manage my time and set boundaries.
+Throughout the sequence of questions, focus on facilitating my thought-processing for deciding next steps by asking follow-up questions and offering further suggestions when appropriate. The goal is to help me be clear on how I can improve my work-life balance and identify meaningful next steps to achieve a healthier work-life balance.</t>
+  </si>
+  <si>
+    <t>Help me identify areas for development and what resources are available to me.
+Ask what I initiatives I have already taken.
+Ask what I am doing to further my learning and skillset.
+Ask what I have been doing to further my network.
+Throughout the sequence of questions, focus on facilitating my thought-processing for deciding next steps by asking follow-up questions and offering further suggestions when appropriate. The goal is to help me identify areas for development, explore relevant resources, and create a meaningful action plan to enhance my skills and stay competitive in my industry and role.</t>
+  </si>
+  <si>
+    <t>Challenge my answers, and discuss my leadership potential.
+Ask what I initiatives I have already taken.
+Explore strategies to grow my leadership skills.
+Ask what I am doing to further my learning and skillset.
+Ask what I have been doing to further my network.
+Throughout the sequence of questions, focus on facilitating my thought-processing for deciding next steps by asking follow-up questions and offering further suggestions when appropriate. The goal is to refine my leadership potential and explore strategies to grow my leadership skills. By the end of our discussion, I should have identified key competencies, target areas for improvement, and have an action plan to excel as a leader.</t>
+  </si>
+  <si>
+    <t>Help me understand how to build a strong personal brand.
+Help me to identify my unique selling points and develop a consistent message.
+Ask what I initiatives I have already taken.
+Ask what I am doing to further promote myself across the business and network.
+Throughout the sequence of questions, focus on facilitating my thought-processing for deciding next steps by asking follow-up questions and offering further suggestions when appropriate. The goal is to help me identify my unique selling points, and create a plan to build a strong personal brand and promote myself effectively across various platforms.</t>
+  </si>
+  <si>
+    <t>Challenge my current performance and help me identify areas for improvement.
+Ask what I initiatives I have already taken.
+Ask what I am doing to enhance my productivity, efficiency and quality work.
+Ask what additional learning I am doing.
+Ask what I have been doing to further my network.
+Throughout the sequence of questions, focus on facilitating my thought-processing for deciding next steps by asking follow-up questions and offering further suggestions when appropriate. The goal is to help me develop a tailored plan to enhance my productivity, efficiency, and overall work quality, setting me up for continued success.</t>
+  </si>
+  <si>
+    <t>Ask what I development programs I have already taken.
+Ask me about my career goals, and help me identify what learning programs would be most appropriate and useful.
+Throughout the sequence of questions, focus on facilitating my thought-processing for deciding next steps by asking follow-up questions and offering further suggestions when appropriate. The goal is to help me identify some AIA development programs to sign up for, and prompt me to take action.</t>
+  </si>
+  <si>
+    <t>Ask me about what habits are working well now, and which could be improved.
+Help me identify the habits that impact my professional and personal life.
+Hep me identify areas for improvement and habits that I should start or stop.
+Throughout the sequence of questions, focus on facilitating my thought-processing for deciding next steps by asking follow-up questions and offering further suggestions when appropriate. The goal is to identify areas for improvement and create a plan to cultivate healthier, more productive habits to support my success.</t>
+  </si>
+  <si>
+    <t>Using inspiration from the book, 'The First 90 Days', ask me questions about my new team and responsibility.
+Guide me through the types of questions I should be asking myself, and what I should be finding out about my new role, manager and team expectations and responsibilities.
+Help me plan action steps to ensure a smooth and successful transition.
+Throughout the sequence of questions, focus on facilitating my thought-processing for deciding next steps by asking follow-up questions and offering further suggestions when appropriate. The goal is to help me create a plan to integrate smoothly into my new responsibilities.</t>
+  </si>
+  <si>
+    <t>Challenge my answers, and ask relevant questions for a deeper understanding.
+Ask what I initiatives I have already taken.
+Ask what I am doing to further my learning and skillset.
+Ask what I have been doing to find other talent.
+Throughout the sequence of questions, focus on facilitating my thought-processing for deciding next steps by asking follow-up questions and offering further suggestions when appropriate. The goal is to help me create a smooth transition plan to ensure continuity and success.</t>
+  </si>
+  <si>
+    <t>Challenge my answers, and ask relevant questions for a deeper understanding.
+Ask what I initiatives I have already taken.
+Ask what I am doing to further my learning and skillset.
+Ask what I have been doing to further my network.
+Throughout the sequence of questions, focus on facilitating my thought-processing for deciding next steps by asking follow-up questions and offering further suggestions when appropriate. The goal is to help me refine why I feel stuck in my role, and help me decide on some meaningful next steps I can take.</t>
+  </si>
+  <si>
+    <t>Career@AIA</t>
+  </si>
+  <si>
+    <t>Let's cover the basics.</t>
+  </si>
+  <si>
+    <t>Thank you for taking the time to explore your career at AIA. We are here to help you clarify and navigate your professional journey within our organisation. Our goal is to provide personalised guidance, and where possible, connect you with resources that help in your current and future roles.
+We encourage you to take advantage of this service, whether you're just starting out, seeking advancement, facing challenges or want to explore new opportunities within the company. Together, let's embark on a journey toward achieving your career goals.
+Any information provided is confidential and will not be shared further.</t>
+  </si>
+  <si>
+    <t>Choose a topic below and share some initial background.</t>
+  </si>
+  <si>
+    <t>intro_prompt</t>
+  </si>
+  <si>
+    <t>Reply with a brief welcome, and share that next we will select a topic to discuss today. No more than 50 words. Do not sign off. Do not ask any questions at this stage.</t>
+  </si>
+  <si>
+    <t>We will work through a series of prompts, designed to guide your thinking, and create actionable steps you can take.
+During our coaching session, please avoid providing any personal information such as address, phone number, date of birth, account details, etc.</t>
+  </si>
+  <si>
+    <t>**Thanks for taking the time to discuss your career today. Below is a summary of our conversation, and some suggested actions steps you can take. As an AI coach, you should use this as guidance, not an absolute directive. You should use your own judgement and consider the advice in the context of your unique situation and goals. Please also check information with reliable sources, especially when making important decisions.**</t>
+  </si>
+  <si>
+    <t>We'll focus on your ongoing professional growth, identify areas for development, explore relevant resources, and create a plan to enhance your skills and stay competitive in your industry.</t>
+  </si>
+  <si>
+    <t>We'll discuss your leadership potential and explore strategies to grow your leadership skills. During this session we identify key competencies, target areas for improvement, and create a plan to help you excel as a leader.</t>
+  </si>
+  <si>
+    <t>We'll discuss your aspirations and purpose. During the session, we identify a career path that resonates with you, set realistic goals and create an action plan.</t>
+  </si>
+  <si>
+    <t>We'll explore your ambitions for promotion and the criteria at AIA. During the session, we'll assess your current skill set, identify areas for growth, and create a plan to help you stand out and advance.</t>
+  </si>
+  <si>
+    <t>We'll discuss the importance of succession planning in your career and organisation. We will evaluate potential successors, discuss how to develop their skills, and create a smooth transition plan to ensure continuity and success.</t>
+  </si>
+  <si>
+    <t>We'll address your feelings of stagnation and explore potential opportunities for growth. During the session, we'll reassess your goals, identify new challenges, and develop a plan to reinvigorate your career journey.</t>
+  </si>
+  <si>
+    <t>We'll address stress and burnout in your professional life. During the session, we'lle xplore the underlying causes, identify coping strategies, and create a plan to enhance your resilience and overall well-being.</t>
+  </si>
+  <si>
+    <t>We'll examine your current role and identify areas where you could be more challenged. During the session, we'll create a plan to discuss these opportunities with your manager and take proactive steps to enhance your job satisfaction.</t>
+  </si>
+  <si>
+    <t>We'll discuss strategies to achieve a healthier work-life balance. During the session, we'll explore time management techniques, set boundaries, and create a plan that supports both your professional and personal well-being.</t>
+  </si>
+  <si>
+    <t>We'll evaluate your current performance and identify areas for improvement. During the session, we'll develop a tailored plan to enhance your productivity, efficiency, and overall work quality, setting you up for continued success.</t>
+  </si>
+  <si>
+    <t>We'll discuss the various AIA development programs available to support your growth. During the session, we'll identify the most suitable programs for your goals and create a plan to maximise the benefits of your participation.</t>
+  </si>
+  <si>
+    <t>We'll explore the habits that impact your professional and personal life. During the session, we'll identify areas for improvement and create a plan to cultivate healthier, more productive habits to support your success.</t>
+  </si>
+  <si>
+    <t>We'll focus on improving your time management skills. During the session, we'll explore various techniques, identify your priorities, and create a personalised plan to optimise your productivity and achieve a better work-life balance.</t>
+  </si>
+  <si>
+    <t>We'll navigate the transition to AIA. During the session, we'll discuss the company culture, expectations, and resources available to support your success, as well as create a plan to help you integrate smoothly into your new role.</t>
+  </si>
+  <si>
+    <t>We'll cover your transition to a new team or role. During the session, we'll help you identify transferable skills, set new goals, and create a plan to adapt to your new responsibilities, ensuring a smooth and successful transition.</t>
+  </si>
+  <si>
+    <t>We'll help you identify transferable skills, set new goals, and create a plan to adapt to your new responsibilities, ensuring a smooth and successful transition.</t>
+  </si>
+  <si>
+    <t>Challenge me and help me refine my career aspirations and objectives.
+Help me identify my purpose, strengths, and values.
+Help me reflect on what i'm good at, self-assess my weaknesses and increase my own awareness.
+Ask what I initiatives I have already taken.
+Ask what I am doing to further my learning and skillset, point me to AIA resources where appropriate.
+Ask what I have been doing to further my network.
+Throughout the sequence of questions, focus on facilitating my thought-processing for deciding next steps by asking follow-up questions and offering further suggestions when appropriate. The goal is to help me refine my career goals, and help me decide on some meaningful next steps I can take.</t>
+  </si>
+  <si>
+    <t>analysis_prompt</t>
+  </si>
+  <si>
+    <t>[Brief introduction, then ask Question 1, provided by you]
+%Answer 1, written by me%
+[150 word or longer reply to Answer 1, then Question 2, provided by you]
+%Answer 2, written by me%
+...
+[150 word or longer reply to Penultimate Answer, then Last Question, provided by you]
+%Last Answer, written by me%
+[150 word or longer reply to Last Answer]</t>
+  </si>
+  <si>
+    <t>Write a 250 word recap of our discussion with goals and suggested action points. The actions should be specific, measurable, achievable, relevant, and time-bound. The actions should clearly define a WHAT and a HOW. Do not add any text after the last action point. The suggested actions should be written in first person (e.g. "I will schedule..."). You can refer me to relevant internal AIA site pages if suitable.
+The summary should follow the format below, where the descriptions in [ ] should be generated by you, and the descriptions between % % will be provided by me. Please use github flavored markdown and use bullets if relevant.
+[Recap of our discussion, key concerns, problems and potential approaches, approximately 200 words]
+#### Action Plan
+Below are some suggestions of actions you can take. You understand your situation best, so please edit and use these as a starting point or create your own. Consider adding these to your PDD goals.
+::Action:: [Suggested Action]
+::Action:: [Suggested Action]
+::Action:: [Suggested Action]</t>
+  </si>
+  <si>
+    <t>Challenge my answers, and ask relevant questions for a deeper understanding.
+Ask what I initiatives I have already taken
+Ask what I am good at and dislike, and what i'm doing to further my learning and skillset, point me to AIA resources where appropriate.
+Ask what I have been doing to further my network.
+- Skills, experience, and impact
+- Interest and demonstrated commitment to learn the skills needed for the next level
+If I tell you I have been passed over for promotion (or similar), remind me that at AIA, promotions are a combination of:
+- Business need for the role at a more senior band. If there is not sufficient business need, AIA may not need to promote employees.
+Throughout the sequence of questions, focus on facilitating my thought-processing for deciding next steps by asking follow-up questions and offering further suggestions when appropriate. The goal is to manage my expectations, and help me decide on some meaningful next steps I can take to increase my chances of promotion.</t>
+  </si>
+  <si>
+    <t>Analyze our conversation from the perspective of AIA, and provide employee insights in a structured format:
+1. Sentiment Analysis - Assign scores (0-100) for the following emotions: Satisfaction, Dissatisfaction, Anger, Fear, Surprise, Discust, Anxiety, Enthusiasm, Boredom, Confidence. Display as a table (Github markdown). Use a standardized methodology, which includes pre-processing, feature extraction, sentiment lexicon or a pre-trained language model, and validation to ensure consistent and reliable sentiment scores.
+2a. Areas for growth and development: Qualitative analysis. 
+2b. Areas for growth and development: Standardised key themes and skill areas.
+3a. Company culture and values alignment: score the level of alignment between employee values and company culture (low, neutral, high)
+3b. Company culture and values alignment: qualitative analysis to help understand the underlying reasons for misalignment's.
+4. Risk of leaving: Quantitative approach. Identifying specific phrases or keywords indicating dissatisfaction or intent to leave can be quantified. (very unlikely, unlikely, neutral, likely, very likely)
+5a. Feedback on company policies and procedures: Qualitative approach. Analyse employee feedback and suggestions. Comparisons can be made by categorizing similar feedback themes across employees.
+5b. Feedback on company policies and procedures: list of key standardised themes.
+6a. Employee goals and aspirations: Qualitative approach. 
+6b. Employee goals and aspirations: List of key standardised themes.
+7. Barriers to success: Qualitative approach. Identify the challenges and obstacles faced by employees. 
+8. Overall satisfaction: Quantitative approach. Employee satisfaction can be measured through standardized survey questions or by analyzing sentiment scores in the conversation. This allows for easy comparison across employees.</t>
   </si>
   <si>
     <t>My name is {user_name}, I am a {band} in {function}. I am {position}.
@@ -451,284 +734,19 @@
 {question_2}
 {reply_2}
 ---
-Taking into consideration the above, guide my thought process through a sequence of questions and proposed answers. Please intitiate the thought-provoking sequence of questions by asking me one question and only ask the next one when an answer is provided. With each question, provide several suggestions.
+Taking into consideration the above, guide my thought process through a sequence of questions and proposed answers. Please intitiate the thought-provoking sequence of questions by asking me one question and only ask the next one when an answer is provided. With each question, ensure it is relevant to my role, and provide several suggestions. Format the question in bold using github flavoured markup.
 {question_guidance}
-The questions should be asked one at a time, only move onto the next question after I have replied. 
+The questions should be asked one at a time, only move onto the next question after I have replied.  
 Ask me exactly {max_questions} questions. 
 Our conversation should progress as follows:
 {question_format}</t>
-  </si>
-  <si>
-    <t>mission</t>
-  </si>
-  <si>
-    <t>### Purpose Statement
-AIA's Purpose is to help people live Healthier, Longer, Better Lives, in every community in which we live and work, with products and policies that don't just protect lives but help make lives healthier, longer and better.</t>
-  </si>
-  <si>
-    <t>mission
-promotions
-learning</t>
-  </si>
-  <si>
-    <t>mission
-learning</t>
-  </si>
-  <si>
-    <t>promotions
-learning
-mission</t>
-  </si>
-  <si>
-    <t>learning
-mental_wellbeing
-mission</t>
-  </si>
-  <si>
-    <t>learning
-promotions
-mission</t>
-  </si>
-  <si>
-    <t>learning
-promotions
-mental_wellbeing
-mission</t>
-  </si>
-  <si>
-    <t>learning
-mental_wellbeing
-promotions
-mission</t>
-  </si>
-  <si>
-    <t>What symptoms of burnout or signs of excessive stress do you experience regularly?</t>
-  </si>
-  <si>
-    <t>Have you identified any areas for improvement in your current role?</t>
-  </si>
-  <si>
-    <t>Are there any specific aspects of leadership you want to improve or develop further?</t>
-  </si>
-  <si>
-    <t>Are there any new habits would you like to develop to improve your overall well-being and success?</t>
-  </si>
-  <si>
-    <t>Challenge my answers, and ask relevant questions for a deeper understanding.
-Help me explore time management techniques and identify my priorities.
-Throughout the sequence of questions, focus on facilitating my thought-processing for deciding next steps by asking follow-up questions and offering further suggestions when appropriate. The goal is to create a personalised action plan to optimise my productivity and achieve a better work life balance.</t>
-  </si>
-  <si>
-    <t>Using inspiration from the book, 'The First 90 Days', ask me questions about my new role and responsibility.
-Guide me through the types of questions I should be asking myself, and what I should be finding out about my new role, manager and responsibilities.
-Throughout the sequence of questions, focus on facilitating my thought-processing for deciding next steps by asking follow-up questions and offering further suggestions when appropriate. The goal is to help me create a plan to integrate smoothly into a new role.</t>
-  </si>
-  <si>
-    <t>Using inspiration from the book, 'The First 90 Days', ask me questions about my new team and responsibility.
-Guide me through the types of questions I should be asking myself, and what I should be finding out about my new role, manager and responsibilities.
-Help me plan action steps to ensure a smooth and successful transition.
-Throughout the sequence of questions, focus on facilitating my thought-processing for deciding next steps by asking follow-up questions and offering further suggestions when appropriate. The goal is to help me create a plan to integrate smoothly into a new role.</t>
-  </si>
-  <si>
-    <t>TBC…</t>
-  </si>
-  <si>
-    <t>We'll understand the process of building a strong personal brand. We'll help you identify your unique selling points, develop a consistent message, and create a plan to promote yourself effectively across various platforms.</t>
-  </si>
-  <si>
-    <t>Help me identify why I'm feeling stressed.
-Challenge why I'm feeling stressed in these situations, ask how I might reframe the situation.
-Ask what symptoms of burnout or signs of excessive stress I have experienced, give some examples.
-Ask what I initiatives I have already taken, and what I'm doing to recover or adapt my workload.
-Ask if I have attended AIA's mental wellbeing workshop, and recommend me to sign up if I have not.
-Throughout the sequence of questions, focus on facilitating my thought-processing for deciding next steps by asking follow-up questions and offering further suggestions when appropriate. The goal is to help me identify some meaningful next steps I can take to reduce, manage and recover from my stress.</t>
-  </si>
-  <si>
-    <t>Challenge my answers, and ask relevant questions for a deeper understanding.
-Ask what I initiatives I have already taken.
-Ask what I am doing to further my learning and skillset.
-Ask if I have discussed with my manager.
-Ask what I have been doing to further my network.
-Throughout the sequence of questions, focus on facilitating my thought-processing for deciding next steps by asking follow-up questions and offering further suggestions when appropriate. The goal is to help me refine why I feel a lack of stimulation or challenge, help me decide on some meaningful next steps I can feel more challenged, create a plan to discuss with my manager and take proactive steps to enhance my job satisfaction.</t>
-  </si>
-  <si>
-    <t>Help me identify what's challenging my work life balance.
-Ask what I initiatives I have already taken to improve it, and what I'm in control of.
-Ask what I am doing to manage my time and set boundaries.
-Throughout the sequence of questions, focus on facilitating my thought-processing for deciding next steps by asking follow-up questions and offering further suggestions when appropriate. The goal is to help me be clear on how I can improve my work-life balance and identify meaningful next steps to achieve a healthier work-life balance.</t>
-  </si>
-  <si>
-    <t>Help me identify areas for development and what resources are available to me.
-Ask what I initiatives I have already taken.
-Ask what I am doing to further my learning and skillset.
-Ask what I have been doing to further my network.
-Throughout the sequence of questions, focus on facilitating my thought-processing for deciding next steps by asking follow-up questions and offering further suggestions when appropriate. The goal is to help me identify areas for development, explore relevant resources, and create a meaningful action plan to enhance my skills and stay competitive in my industry and role.</t>
-  </si>
-  <si>
-    <t>Challenge my answers, and discuss my leadership potential.
-Ask what I initiatives I have already taken.
-Explore strategies to grow my leadership skills.
-Ask what I am doing to further my learning and skillset.
-Ask what I have been doing to further my network.
-Throughout the sequence of questions, focus on facilitating my thought-processing for deciding next steps by asking follow-up questions and offering further suggestions when appropriate. The goal is to refine my leadership potential and explore strategies to grow my leadership skills. By the end of our discussion, I should have identified key competencies, target areas for improvement, and have an action plan to excel as a leader.</t>
-  </si>
-  <si>
-    <t>Help me understand how to build a strong personal brand.
-Help me to identify my unique selling points and develop a consistent message.
-Ask what I initiatives I have already taken.
-Ask what I am doing to further promote myself across the business and network.
-Throughout the sequence of questions, focus on facilitating my thought-processing for deciding next steps by asking follow-up questions and offering further suggestions when appropriate. The goal is to help me identify my unique selling points, and create a plan to build a strong personal brand and promote myself effectively across various platforms.</t>
-  </si>
-  <si>
-    <t>Challenge my current performance and help me identify areas for improvement.
-Ask what I initiatives I have already taken.
-Ask what I am doing to enhance my productivity, efficiency and quality work.
-Ask what additional learning I am doing.
-Ask what I have been doing to further my network.
-Throughout the sequence of questions, focus on facilitating my thought-processing for deciding next steps by asking follow-up questions and offering further suggestions when appropriate. The goal is to help me develop a tailored plan to enhance my productivity, efficiency, and overall work quality, setting me up for continued success.</t>
-  </si>
-  <si>
-    <t>Ask what I development programs I have already taken.
-Ask me about my career goals, and help me identify what learning programs would be most appropriate and useful.
-Throughout the sequence of questions, focus on facilitating my thought-processing for deciding next steps by asking follow-up questions and offering further suggestions when appropriate. The goal is to help me identify some AIA development programs to sign up for, and prompt me to take action.</t>
-  </si>
-  <si>
-    <t>Ask me about what habits are working well now, and which could be improved.
-Help me identify the habits that impact my professional and personal life.
-Hep me identify areas for improvement and habits that I should start or stop.
-Throughout the sequence of questions, focus on facilitating my thought-processing for deciding next steps by asking follow-up questions and offering further suggestions when appropriate. The goal is to identify areas for improvement and create a plan to cultivate healthier, more productive habits to support my success.</t>
-  </si>
-  <si>
-    <t>Using inspiration from the book, 'The First 90 Days', ask me questions about my new team and responsibility.
-Guide me through the types of questions I should be asking myself, and what I should be finding out about my new role, manager and team expectations and responsibilities.
-Help me plan action steps to ensure a smooth and successful transition.
-Throughout the sequence of questions, focus on facilitating my thought-processing for deciding next steps by asking follow-up questions and offering further suggestions when appropriate. The goal is to help me create a plan to integrate smoothly into my new responsibilities.</t>
-  </si>
-  <si>
-    <t>Challenge my answers, and ask relevant questions for a deeper understanding.
-Ask what I initiatives I have already taken.
-Ask what I am doing to further my learning and skillset.
-Ask what I have been doing to find other talent.
-Throughout the sequence of questions, focus on facilitating my thought-processing for deciding next steps by asking follow-up questions and offering further suggestions when appropriate. The goal is to help me create a smooth transition plan to ensure continuity and success.</t>
-  </si>
-  <si>
-    <t>Challenge my answers, and ask relevant questions for a deeper understanding.
-Ask what I initiatives I have already taken.
-Ask what I am doing to further my learning and skillset.
-Ask what I have been doing to further my network.
-Throughout the sequence of questions, focus on facilitating my thought-processing for deciding next steps by asking follow-up questions and offering further suggestions when appropriate. The goal is to help me refine why I feel stuck in my role, and help me decide on some meaningful next steps I can take.</t>
-  </si>
-  <si>
-    <t>Career@AIA</t>
-  </si>
-  <si>
-    <t>Let's cover the basics.</t>
-  </si>
-  <si>
-    <t>Thank you for taking the time to explore your career at AIA. We are here to help you clarify and navigate your professional journey within our organisation. Our goal is to provide personalised guidance, and where possible, connect you with resources that help in your current and future roles.
-We encourage you to take advantage of this service, whether you're just starting out, seeking advancement, facing challenges or want to explore new opportunities within the company. Together, let's embark on a journey toward achieving your career goals.
-Any information provided is confidential and will not be shared further.</t>
-  </si>
-  <si>
-    <t>Choose a topic below and share some initial background.</t>
-  </si>
-  <si>
-    <t>intro_prompt</t>
-  </si>
-  <si>
-    <t>Reply with a brief welcome, and share that next we will select a topic to discuss today. No more than 50 words. Do not sign off. Do not ask any questions at this stage.</t>
-  </si>
-  <si>
-    <t>We will work through a series of prompts, designed to guide your thinking, and create actionable steps you can take.
-During our coaching session, please avoid providing any personal information such as address, phone number, date of birth, account details, etc.</t>
-  </si>
-  <si>
-    <t>**Thanks for taking the time to discuss your career today. Below is a summary of our conversation, and some suggested actions steps you can take. As an AI coach, you should use this as guidance, not an absolute directive. You should use your own judgement and consider the advice in the context of your unique situation and goals. Please also check information with reliable sources, especially when making important decisions.**</t>
-  </si>
-  <si>
-    <t>We'll focus on your ongoing professional growth, identify areas for development, explore relevant resources, and create a plan to enhance your skills and stay competitive in your industry.</t>
-  </si>
-  <si>
-    <t>We'll discuss your leadership potential and explore strategies to grow your leadership skills. During this session we identify key competencies, target areas for improvement, and create a plan to help you excel as a leader.</t>
-  </si>
-  <si>
-    <t>We'll discuss your aspirations and purpose. During the session, we identify a career path that resonates with you, set realistic goals and create an action plan.</t>
-  </si>
-  <si>
-    <t>We'll explore your ambitions for promotion and the criteria at AIA. During the session, we'll assess your current skill set, identify areas for growth, and create a plan to help you stand out and advance.</t>
-  </si>
-  <si>
-    <t>We'll discuss the importance of succession planning in your career and organisation. We will evaluate potential successors, discuss how to develop their skills, and create a smooth transition plan to ensure continuity and success.</t>
-  </si>
-  <si>
-    <t>We'll address your feelings of stagnation and explore potential opportunities for growth. During the session, we'll reassess your goals, identify new challenges, and develop a plan to reinvigorate your career journey.</t>
-  </si>
-  <si>
-    <t>We'll address stress and burnout in your professional life. During the session, we'lle xplore the underlying causes, identify coping strategies, and create a plan to enhance your resilience and overall well-being.</t>
-  </si>
-  <si>
-    <t>We'll examine your current role and identify areas where you could be more challenged. During the session, we'll create a plan to discuss these opportunities with your manager and take proactive steps to enhance your job satisfaction.</t>
-  </si>
-  <si>
-    <t>We'll discuss strategies to achieve a healthier work-life balance. During the session, we'll explore time management techniques, set boundaries, and create a plan that supports both your professional and personal well-being.</t>
-  </si>
-  <si>
-    <t>We'll evaluate your current performance and identify areas for improvement. During the session, we'll develop a tailored plan to enhance your productivity, efficiency, and overall work quality, setting you up for continued success.</t>
-  </si>
-  <si>
-    <t>We'll discuss the various AIA development programs available to support your growth. During the session, we'll identify the most suitable programs for your goals and create a plan to maximise the benefits of your participation.</t>
-  </si>
-  <si>
-    <t>We'll explore the habits that impact your professional and personal life. During the session, we'll identify areas for improvement and create a plan to cultivate healthier, more productive habits to support your success.</t>
-  </si>
-  <si>
-    <t>We'll focus on improving your time management skills. During the session, we'll explore various techniques, identify your priorities, and create a personalised plan to optimise your productivity and achieve a better work-life balance.</t>
-  </si>
-  <si>
-    <t>We'll navigate the transition to AIA. During the session, we'll discuss the company culture, expectations, and resources available to support your success, as well as create a plan to help you integrate smoothly into your new role.</t>
-  </si>
-  <si>
-    <t>We'll cover your transition to a new team or role. During the session, we'll help you identify transferable skills, set new goals, and create a plan to adapt to your new responsibilities, ensuring a smooth and successful transition.</t>
-  </si>
-  <si>
-    <t>We'll help you identify transferable skills, set new goals, and create a plan to adapt to your new responsibilities, ensuring a smooth and successful transition.</t>
-  </si>
-  <si>
-    <t>[Brief introduction, then ask Question 1, provided by you]
-%Answer 1, written by me%
-[150 word or longer reply to Answer 1, then Question 2, provided by you]
-%Answer 2, written by me%
-...
-[150 word or longer reply to Answer N-1, then Question N, provided by you]
-%Answer N, written by me%
-[150 word or longer reply to Answer N]</t>
-  </si>
-  <si>
-    <t>Challenge my answers, and ask relevant questions for a deeper understanding.
-Ask what I initiatives I have already taken.
-Ask what I am good at and dislike, and what i'm doing to further my learning and skillset, point me to AIA resources where appropriate.
-Ask what I have been doing to further my network.
-- Skills, experience, and impact
-- Interest and demonstrated commitment to learn the skills needed for the next level
-If I tell you I have been passed over for promotion (or similar), remind me that at AIA, promotions are a combination of:
-- Business need for the role at a more senior band. If there is not sufficient business need, AIA may not need to promote employees.
-Throughout the sequence of questions, focus on facilitating my thought-processing for deciding next steps by asking follow-up questions and offering further suggestions when appropriate. The goal is to manage my expectations, and help me decide on some meaningful next steps I can take to increase my chances of promotion.</t>
-  </si>
-  <si>
-    <t>Challenge me and help me refine my career aspirations and objectives.
-Help me identify my purpose, strengths, and values.
-Help me reflect on what i'm good at, self-assess my weaknesses and increase my own awareness.
-Ask what I initiatives I have already taken.
-Ask what I am doing to further my learning and skillset, point me to AIA resources where appropriate.
-Ask what I have been doing to further my network.
-Throughout the sequence of questions, focus on facilitating my thought-processing for deciding next steps by asking follow-up questions and offering further suggestions when appropriate. The goal is to help me refine my career goals, and help me decide on some meaningful next steps I can take.</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -752,6 +770,12 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF260000"/>
+      <name val="Source Sans Pro"/>
+      <family val="2"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -774,7 +798,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="18">
+  <cellXfs count="19">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center"/>
@@ -825,6 +849,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -841,10 +866,6 @@
     </ext>
   </extLst>
 </styleSheet>
-</file>
-
-<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
-<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1144,10 +1165,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CC1EC875-F3B4-48F0-8EAB-93E899189853}">
-  <dimension ref="A1:C9"/>
+  <dimension ref="A1:C10"/>
   <sheetViews>
-    <sheetView topLeftCell="A5" workbookViewId="0">
-      <selection activeCell="B6" sqref="B6"/>
+    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1179,10 +1200,10 @@
     </row>
     <row r="3" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A3" s="1" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
       <c r="C3" s="1"/>
     </row>
@@ -1191,7 +1212,7 @@
         <v>77</v>
       </c>
       <c r="B4" s="6" t="s">
-        <v>123</v>
+        <v>182</v>
       </c>
       <c r="C4" s="1"/>
     </row>
@@ -1204,19 +1225,31 @@
       </c>
       <c r="C5" s="1"/>
     </row>
-    <row r="6" spans="1:3" ht="316.8" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:3" ht="331.2" x14ac:dyDescent="0.3">
       <c r="A6" s="1" t="s">
         <v>23</v>
       </c>
       <c r="B6" s="5" t="s">
-        <v>100</v>
+        <v>179</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" ht="409.6" x14ac:dyDescent="0.3">
+      <c r="A7" s="1" t="s">
+        <v>177</v>
+      </c>
+      <c r="B7" s="5" t="s">
+        <v>181</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.3">
       <c r="B9" s="5"/>
     </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="B10" s="18"/>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -1224,9 +1257,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{91B67F92-929D-4748-A060-6C905D3C4127}">
   <dimension ref="A1:E9"/>
   <sheetViews>
-    <sheetView topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="D4" sqref="D4"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
@@ -1258,13 +1289,13 @@
         <v>0</v>
       </c>
       <c r="B2" s="16" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
       <c r="C2" s="2" t="s">
         <v>4</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>156</v>
+        <v>154</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.3">
@@ -1275,7 +1306,7 @@
         <v>2</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
       <c r="D3" s="2" t="s">
         <v>5</v>
@@ -1297,10 +1328,10 @@
         <v>83</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
       <c r="D5" s="2" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.3">
@@ -1316,13 +1347,13 @@
         <v>96</v>
       </c>
       <c r="B7" s="16" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
       <c r="C7" s="2" t="s">
         <v>97</v>
       </c>
       <c r="D7" s="2" t="s">
-        <v>161</v>
+        <v>159</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.3">
@@ -1351,7 +1382,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5990ADE6-0F99-4D0A-96A1-792BDD041915}">
   <dimension ref="A1:B15"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A3" sqref="A3"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
@@ -1555,11 +1588,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DCC4B99F-D286-4F78-BAC8-23AC2E322EDE}">
   <dimension ref="A1:I26"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="C2" activePane="bottomRight" state="frozen"/>
+    <sheetView workbookViewId="0">
+      <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="C5" sqref="C5"/>
+      <selection pane="bottomRight" activeCell="A6" sqref="A6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1588,7 +1621,7 @@
         <v>42</v>
       </c>
       <c r="E1" s="11" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="F1" s="11" t="s">
         <v>41</v>
@@ -1623,19 +1656,19 @@
         <v>57</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>164</v>
+        <v>162</v>
       </c>
       <c r="C4" s="6" t="s">
-        <v>180</v>
+        <v>176</v>
       </c>
       <c r="D4" s="9">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="E4" s="2" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="G4" s="2" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
       <c r="H4" s="1"/>
     </row>
@@ -1644,19 +1677,19 @@
         <v>52</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
       <c r="C5" s="6" t="s">
-        <v>179</v>
+        <v>180</v>
       </c>
       <c r="D5" s="9">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="E5" s="2" t="s">
         <v>66</v>
       </c>
       <c r="G5" s="2" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
       <c r="H5" s="1"/>
     </row>
@@ -1665,19 +1698,19 @@
         <v>20</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>166</v>
+        <v>164</v>
       </c>
       <c r="C6" s="6" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
       <c r="D6" s="9">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="E6" s="2" t="s">
         <v>67</v>
       </c>
       <c r="G6" s="2" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
       <c r="H6" s="1"/>
     </row>
@@ -1695,20 +1728,20 @@
         <v>58</v>
       </c>
       <c r="B8" s="6" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
       <c r="C8" s="6" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
       <c r="D8" s="9">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="E8" s="6" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="F8" s="6"/>
       <c r="G8" s="6" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
       <c r="H8" s="1"/>
       <c r="I8" s="5"/>
@@ -1718,22 +1751,22 @@
         <v>59</v>
       </c>
       <c r="B9" s="2" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
       <c r="C9" s="6" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
       <c r="D9" s="9">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="E9" s="6" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="F9" s="6" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="G9" s="6" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
       <c r="H9" s="1"/>
       <c r="I9" s="5"/>
@@ -1743,20 +1776,20 @@
         <v>82</v>
       </c>
       <c r="B10" s="2" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
       <c r="C10" s="6" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
       <c r="D10" s="9">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="E10" s="6" t="s">
         <v>68</v>
       </c>
       <c r="F10" s="6"/>
       <c r="G10" s="6" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
       <c r="H10" s="1"/>
       <c r="I10" s="5"/>
@@ -1766,22 +1799,22 @@
         <v>81</v>
       </c>
       <c r="B11" s="2" t="s">
-        <v>170</v>
+        <v>168</v>
       </c>
       <c r="C11" s="6" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
       <c r="D11" s="9">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="E11" s="6" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="F11" s="6" t="s">
         <v>69</v>
       </c>
       <c r="G11" s="6" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
       <c r="H11" s="1"/>
       <c r="I11" s="5"/>
@@ -1803,22 +1836,22 @@
         <v>18</v>
       </c>
       <c r="B13" s="2" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
       <c r="C13" s="6" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
       <c r="D13" s="9">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="E13" s="6" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
       <c r="F13" s="6" t="s">
         <v>70</v>
       </c>
       <c r="G13" s="6" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
       <c r="H13" s="1"/>
       <c r="I13" s="5"/>
@@ -1828,20 +1861,20 @@
         <v>19</v>
       </c>
       <c r="B14" s="2" t="s">
-        <v>163</v>
+        <v>161</v>
       </c>
       <c r="C14" s="6" t="s">
-        <v>146</v>
+        <v>144</v>
       </c>
       <c r="D14" s="9">
         <v>4</v>
       </c>
       <c r="E14" s="6" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
       <c r="F14" s="6"/>
       <c r="G14" s="6" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
       <c r="H14" s="1"/>
       <c r="I14" s="5"/>
@@ -1851,22 +1884,22 @@
         <v>54</v>
       </c>
       <c r="B15" s="2" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
       <c r="C15" s="6" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
       <c r="D15" s="9">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="E15" s="6" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="F15" s="6" t="s">
         <v>71</v>
       </c>
       <c r="G15" s="6" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
       <c r="H15" s="1"/>
       <c r="I15" s="5"/>
@@ -1876,22 +1909,22 @@
         <v>60</v>
       </c>
       <c r="B16" s="2" t="s">
-        <v>171</v>
+        <v>169</v>
       </c>
       <c r="C16" s="6" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
       <c r="D16" s="9">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="E16" s="6" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="F16" s="6" t="s">
         <v>72</v>
       </c>
       <c r="G16" s="6" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
       <c r="H16" s="1"/>
       <c r="I16" s="5"/>
@@ -1901,20 +1934,20 @@
         <v>49</v>
       </c>
       <c r="B17" s="2" t="s">
-        <v>172</v>
+        <v>170</v>
       </c>
       <c r="C17" s="6" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
       <c r="D17" s="9">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="E17" s="6" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="F17" s="6"/>
       <c r="G17" s="6" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
       <c r="H17" s="1"/>
       <c r="I17" s="5"/>
@@ -1924,22 +1957,22 @@
         <v>61</v>
       </c>
       <c r="B18" s="2" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
       <c r="C18" s="6" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
       <c r="D18" s="9">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="E18" s="6" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="F18" s="6" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
       <c r="G18" s="2" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
       <c r="H18" s="1"/>
       <c r="I18" s="5"/>
@@ -1949,22 +1982,22 @@
         <v>56</v>
       </c>
       <c r="B19" s="2" t="s">
-        <v>174</v>
+        <v>172</v>
       </c>
       <c r="C19" s="6" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
       <c r="D19" s="9">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="E19" s="6" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="F19" s="6" t="s">
         <v>73</v>
       </c>
       <c r="G19" s="2" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
       <c r="H19" s="1"/>
       <c r="I19" s="5"/>
@@ -1986,20 +2019,20 @@
         <v>63</v>
       </c>
       <c r="B21" s="7" t="s">
-        <v>175</v>
+        <v>173</v>
       </c>
       <c r="C21" s="6" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
       <c r="D21" s="9">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="E21" s="6" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="F21" s="6"/>
       <c r="G21" s="2" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
       <c r="H21" s="1"/>
       <c r="I21" s="5"/>
@@ -2009,22 +2042,22 @@
         <v>62</v>
       </c>
       <c r="B22" s="2" t="s">
-        <v>176</v>
+        <v>174</v>
       </c>
       <c r="C22" s="6" t="s">
-        <v>139</v>
+        <v>137</v>
       </c>
       <c r="D22" s="9">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="E22" s="6" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="F22" s="6" t="s">
         <v>74</v>
       </c>
       <c r="G22" s="2" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
       <c r="H22" s="1"/>
       <c r="I22" s="5"/>
@@ -2034,22 +2067,22 @@
         <v>64</v>
       </c>
       <c r="B23" s="2" t="s">
-        <v>177</v>
+        <v>175</v>
       </c>
       <c r="C23" s="6" t="s">
-        <v>151</v>
+        <v>149</v>
       </c>
       <c r="D23" s="9">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="E23" s="2" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="F23" s="2" t="s">
         <v>75</v>
       </c>
       <c r="G23" s="2" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
       <c r="H23" s="1"/>
     </row>
@@ -2064,21 +2097,21 @@
     </row>
     <row r="25" spans="1:9" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A25" s="12" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
       <c r="B25" s="2"/>
       <c r="C25" s="6"/>
       <c r="D25" s="9">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="E25" s="2" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="F25" s="2" t="s">
         <v>76</v>
       </c>
       <c r="G25" s="2" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
       <c r="H25" s="1"/>
     </row>
@@ -2105,42 +2138,42 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A1" s="3" t="s">
+        <v>100</v>
+      </c>
+      <c r="B1" s="17" t="s">
         <v>101</v>
-      </c>
-      <c r="B1" s="17" t="s">
-        <v>102</v>
       </c>
     </row>
     <row r="2" spans="1:2" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="B2" s="5" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
     </row>
     <row r="3" spans="1:2" ht="409.6" x14ac:dyDescent="0.3">
       <c r="A3" s="1" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
     </row>
     <row r="4" spans="1:2" ht="115.2" x14ac:dyDescent="0.3">
       <c r="A4" s="1" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
     </row>
     <row r="5" spans="1:2" ht="72" x14ac:dyDescent="0.3">
       <c r="A5" s="1" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Changed Company to AIA
</commit_message>
<xml_diff>
--- a/data.xlsx
+++ b/data.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/7a174a4e09cb8396/1. Projects/pythonCourse/template/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="10" documentId="13_ncr:1_{66D05300-D3C3-44CE-BAEA-3361A0E58396}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{2B19A6D1-E50B-4BA9-A024-D5BC57EE563F}"/>
+  <xr:revisionPtr revIDLastSave="11" documentId="13_ncr:1_{66D05300-D3C3-44CE-BAEA-3361A0E58396}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{91D6A09E-5973-4BBE-BEF2-F77B5BACB9D7}"/>
   <bookViews>
-    <workbookView xWindow="2304" yWindow="2304" windowWidth="25200" windowHeight="14400" xr2:uid="{9AEA82DC-1007-464E-9B9C-0501EEC6530D}"/>
+    <workbookView xWindow="1920" yWindow="1920" windowWidth="25200" windowHeight="14400" xr2:uid="{9AEA82DC-1007-464E-9B9C-0501EEC6530D}"/>
   </bookViews>
   <sheets>
     <sheet name="prompts" sheetId="1" r:id="rId1"/>
@@ -596,103 +596,6 @@
     <t>We'll explore your ambitions for promotion and the criteria. During the session, we'll assess your current skill set, identify areas for growth, and create a plan to help you stand out and advance.</t>
   </si>
   <si>
-    <t>You are an internal career coach at Company. Your aim is to guide me to identify specfic areas of personal and professional development to meet my short and long-term career aspirations, in Company or elsewhere. Your tone should be professional, friendly and empathetic. Use UK english.</t>
-  </si>
-  <si>
-    <t>Write a 250 word recap of our discussion with goals and suggested action points. The actions should be specific, measurable, achievable, relevant, and time-bound. The actions should clearly define a WHAT and a HOW. Do not add any text after the last action point. The suggested actions should be written in first person (e.g. "I will schedule..."). You can refer me to relevant internal Company site pages if suitable.
-The summary should follow the format below, where the descriptions in [ ] should be generated by you, and the descriptions between % % will be provided by me. Please use github flavored markdown and use bullets if relevant.
-[Recap of our discussion, key concerns, problems and potential approaches, approximately 200 words]
-#### Action Plan
-Below are some suggestions of actions you can take. You understand your situation best, so please edit and use these as a starting point or create your own. Consider adding these to your PDD goals.
-::Action:: [Suggested Action]
-::Action:: [Suggested Action]
-::Action:: [Suggested Action]</t>
-  </si>
-  <si>
-    <t>Analyze our conversation from the perspective of Company, and provide employee insights in a structured format:
-1. Sentiment Analysis - Assign scores (0-100) for the following emotions: Satisfaction, Dissatisfaction, Anger, Fear, Surprise, Discust, Anxiety, Enthusiasm, Boredom, Confidence. Display as a table (Github markdown). Use a standardized methodology, which includes pre-processing, feature extraction, sentiment lexicon or a pre-trained language model, and validation to ensure consistent and reliable sentiment scores.
-2a. Areas for growth and development: Qualitative analysis. 
-2b. Areas for growth and development: Standardised key themes and skill areas.
-3a. Company culture and values alignment: score the level of alignment between employee values and company culture (low, neutral, high)
-3b. Company culture and values alignment: qualitative analysis to help understand the underlying reasons for misalignment's.
-4. Risk of leaving: Quantitative approach. Identifying specific phrases or keywords indicating dissatisfaction or intent to leave can be quantified. (very unlikely, unlikely, neutral, likely, very likely)
-5a. Feedback on company policies and procedures: Qualitative approach. Analyse employee feedback and suggestions. Comparisons can be made by categorizing similar feedback themes across employees.
-5b. Feedback on company policies and procedures: list of key standardised themes.
-6a. Employee goals and aspirations: Qualitative approach. 
-6b. Employee goals and aspirations: List of key standardised themes.
-7. Barriers to success: Qualitative approach. Identify the challenges and obstacles faced by employees. 
-8. Overall satisfaction: Quantitative approach. Employee satisfaction can be measured through standardized survey questions or by analyzing sentiment scores in the conversation. This allows for easy comparison across employees.</t>
-  </si>
-  <si>
-    <t>Career@Company</t>
-  </si>
-  <si>
-    <t>Thank you for taking the time to explore your career at Company. We are here to help you clarify and navigate your professional journey within our organisation. Our goal is to provide personalised guidance, and where possible, connect you with resources that help in your current and future roles.
-We encourage you to take advantage of this service, whether you're just starting out, seeking advancement, facing challenges or want to explore new opportunities within the company. Together, let's embark on a journey toward achieving your career goals.
-Any information provided is confidential and will not be shared further.</t>
-  </si>
-  <si>
-    <t>I safeguard Company's financial wellbeing by ensuring our products are well-designed and suitably priced. I also analyse business performance to ensure proper management of the insurance policies in-force, while maintaining adequate reserves, reinsurance and capital levels to fulfil our obligations to policyholders.</t>
-  </si>
-  <si>
-    <t>I support and develop Company's Premier Agency channel through programmes designed to raise the productivity and professionalism of our agency service.</t>
-  </si>
-  <si>
-    <t>I safeguard Company’s financial interests through effective financial controls, timely and accurate management information and insightful financial analysis to support and drive the business forward. I am also responsible for all external reporting including statutory and regulatory filings.</t>
-  </si>
-  <si>
-    <t>I help Company to engage in a meaningful manner with customers and other stakeholders. I ensure the consistency of Company’s messaging across all channels, design marketing campaigns to manage customer advocacy and experience, and use data insights to make key business decisions.</t>
-  </si>
-  <si>
-    <t>I collaborate and partner with banks, independent financial advisory firms, brokerage bodies and other third-party intermediates, to market Company products through various distribution channels.</t>
-  </si>
-  <si>
-    <t>Challenge my answers, and ask relevant questions for a deeper understanding.
-Ask what I initiatives I have already taken.
-Ask what i'm doing to further my learning and skillset, point me to Company resources where appropriate.
-Ask what I have been doing to further my network.
-If I tell you I have been passed over for promotion (or similar), remind me that at Company, promotions are a combination of:
-- Business need for the role at a more senior band. If there is not sufficient business need, Company may not need to promote employees.
-- Skills, experience, and impact
-- Interest and demonstrated commitment to learn the skills needed for the next level
-Throughout the sequence of questions, focus on facilitating my thought-processing for deciding next steps by asking follow-up questions and offering further suggestions when appropriate. The goal is to manage my expectations, and help me decide on some meaningful next steps I can take to increase my chances of promotion.</t>
-  </si>
-  <si>
-    <t>Help me identify why I'm feeling stressed.
-Challenge why I'm feeling stressed in these situations, ask how I might reframe the situation.
-Ask what symptoms of burnout or signs of excessive stress I have experienced, give some examples.
-Ask what I initiatives I have already taken, and what I'm doing to recover or adapt my workload.
-Ask if I have attended Company's mental wellbeing workshop, and recommend me to sign up if I have not.
-Throughout the sequence of questions, focus on facilitating my thought-processing for deciding next steps by asking follow-up questions and offering further suggestions when appropriate. The goal is to help me identify some meaningful next steps I can take to reduce, manage and recover from my stress.</t>
-  </si>
-  <si>
-    <t>Company development programs</t>
-  </si>
-  <si>
-    <t>We'll discuss the various Company development programs available to support your growth. During the session, we'll identify the most suitable programs for your goals and create a plan to maximise the benefits of your participation.</t>
-  </si>
-  <si>
-    <t>Ask what I development programs I have already taken.
-Ask me about my career goals, and help me identify what learning programs would be most appropriate and useful.
-Throughout the sequence of questions, focus on facilitating my thought-processing for deciding next steps by asking follow-up questions and offering further suggestions when appropriate. The goal is to help me identify some Company development programs to sign up for, and prompt me to take action.</t>
-  </si>
-  <si>
-    <t>Do you have any specific career goals and areas for development within Company?</t>
-  </si>
-  <si>
-    <t>Joining Company</t>
-  </si>
-  <si>
-    <t>We'll navigate the transition to Company. During the session, we'll discuss the company culture, expectations, and resources available to support your success, as well as create a plan to help you integrate smoothly into your new role.</t>
-  </si>
-  <si>
-    <t>What is your new role within Company and what are your key responsibilities?</t>
-  </si>
-  <si>
-    <t>### Purpose Statement
-Company's Purpose is to help people live Healthier, Longer, Better Lives, in every community in which we live and work, with products and policies that don't just protect lives but help make lives healthier, longer and better.</t>
-  </si>
-  <si>
     <t>My name is {user_name}, I am a {band} in {function}. I am {position}.
 I have the following experience:
 {experience}
@@ -716,19 +619,6 @@
 {question_format}</t>
   </si>
   <si>
-    <t>#### Learning
-Our learning culture actively supports people in their current roles, while providing a platform for growth and development within Company. Our focus on learning is a key part of our ambition to ensure our people can upskill, reskill, work more flexibly and adapt to the changing world of work. We take a holistic approach to learning and development that includes knowledge and skills accumulated from on-the-job experiences, mobility, collaborative projects, structured virtual lessons and digital self-leaming, supported by mentoring and coaching. 
-We believe that career mobility and assignments in different business units or functions provide our employees with new opportunities. These assignments serve as platforms to learn new skills and help develop the individual's Company network. 
-To ensure that we continue to develop talent for the future, we continuously research the skills and knowledge requirements of our industry and review feedback from our employees, to design the programmes that address these needs. In addition, our people are required to regularly complete mandatory training on a range of technical, governance and conduct-related topics. 
-We have launched, and are in the process of designing additional programmes to incubate new talent capabilities and upskill employees in core lines of business across the Group including the Company Analytics Academy which focuses on building data analytics and business analysis capability across all levels in Company. The "Converge' learning journey is a bespoke 10-month reskilling programme with apprenticeship opportunities for employees to equip them for business analysis roles. 
-We also upskill senior leaders with a stronger understanding of the power of analytics through the "Analytics for Leaders" programme. The Company Agile Academy, which currently provides two reskilling programmes — the "Agile Practitioner" and the "Agile Team Lead" — to help Company build internal capability to drive business transformation. The Company Distribution Leadership Programme, which provides a platform for our most senior distribution leaders to further develop their distribution skill sets. 
-Digital content and delivery methods play an important role in shaping a culture of continuous learning at Company. All our business units provide employees with access to the Company Learning Hub, an online platform which provides access to thousands of digital learning courses. In 2022, we curated digital learning programmes with over 110 modules to support learning needs of employees in management and specialist career tracks. 
-Company Learning Hub can be accessed at www.company.com/learninghub.
-You can sign up for 'Agile Team Lead' here www.company.com/agile-sign-up
-You can sign up for 'Agile Practitioner' here www.company.com/agile-sign-up
-You can sign up for 'Company Distribution Leadership' here www.company.com/distro_leader_sign-up</t>
-  </si>
-  <si>
     <t>### Promotions
 Promotions are a combination of:
 - Business need for the role at a more senior band
@@ -737,8 +627,118 @@
 Promotion criteria is available here: www.company.com/promotion_criteria</t>
   </si>
   <si>
+    <t>You are an internal career coach at AIA. Your aim is to guide me to identify specfic areas of personal and professional development to meet my short and long-term career aspirations, in AIA or elsewhere. Your tone should be professional, friendly and empathetic. Use UK english.</t>
+  </si>
+  <si>
+    <t>Write a 250 word recap of our discussion with goals and suggested action points. The actions should be specific, measurable, achievable, relevant, and time-bound. The actions should clearly define a WHAT and a HOW. Do not add any text after the last action point. The suggested actions should be written in first person (e.g. "I will schedule..."). You can refer me to relevant internal AIA site pages if suitable.
+The summary should follow the format below, where the descriptions in [ ] should be generated by you, and the descriptions between % % will be provided by me. Please use github flavored markdown and use bullets if relevant.
+[Recap of our discussion, key concerns, problems and potential approaches, approximately 200 words]
+#### Action Plan
+Below are some suggestions of actions you can take. You understand your situation best, so please edit and use these as a starting point or create your own. Consider adding these to your PDD goals.
+::Action:: [Suggested Action]
+::Action:: [Suggested Action]
+::Action:: [Suggested Action]</t>
+  </si>
+  <si>
+    <t>Analyze our conversation from the perspective of AIA, and provide employee insights in a structured format:
+1. Sentiment Analysis - Assign scores (0-100) for the following emotions: Satisfaction, Dissatisfaction, Anger, Fear, Surprise, Discust, Anxiety, Enthusiasm, Boredom, Confidence. Display as a table (Github markdown). Use a standardized methodology, which includes pre-processing, feature extraction, sentiment lexicon or a pre-trained language model, and validation to ensure consistent and reliable sentiment scores.
+2a. Areas for growth and development: Qualitative analysis. 
+2b. Areas for growth and development: Standardised key themes and skill areas.
+3a. AIA culture and values alignment: score the level of alignment between employee values and company culture (low, neutral, high)
+3b. AIA culture and values alignment: qualitative analysis to help understand the underlying reasons for misalignment's.
+4. Risk of leaving: Quantitative approach. Identifying specific phrases or keywords indicating dissatisfaction or intent to leave can be quantified. (very unlikely, unlikely, neutral, likely, very likely)
+5a. Feedback on company policies and procedures: Qualitative approach. Analyse employee feedback and suggestions. Comparisons can be made by categorizing similar feedback themes across employees.
+5b. Feedback on company policies and procedures: list of key standardised themes.
+6a. Employee goals and aspirations: Qualitative approach. 
+6b. Employee goals and aspirations: List of key standardised themes.
+7. Barriers to success: Qualitative approach. Identify the challenges and obstacles faced by employees. 
+8. Overall satisfaction: Quantitative approach. Employee satisfaction can be measured through standardized survey questions or by analyzing sentiment scores in the conversation. This allows for easy comparison across employees.</t>
+  </si>
+  <si>
+    <t>Career@AIA</t>
+  </si>
+  <si>
+    <t>Thank you for taking the time to explore your career at AIA. We are here to help you clarify and navigate your professional journey within our organisation. Our goal is to provide personalised guidance, and where possible, connect you with resources that help in your current and future roles.
+We encourage you to take advantage of this service, whether you're just starting out, seeking advancement, facing challenges or want to explore new opportunities within the company. Together, let's embark on a journey toward achieving your career goals.
+Any information provided is confidential and will not be shared further.</t>
+  </si>
+  <si>
+    <t>I safeguard AIA's financial wellbeing by ensuring our products are well-designed and suitably priced. I also analyse business performance to ensure proper management of the insurance policies in-force, while maintaining adequate reserves, reinsurance and capital levels to fulfil our obligations to policyholders.</t>
+  </si>
+  <si>
+    <t>I support and develop AIA's Premier Agency channel through programmes designed to raise the productivity and professionalism of our agency service.</t>
+  </si>
+  <si>
+    <t>I safeguard AIA’s financial interests through effective financial controls, timely and accurate management information and insightful financial analysis to support and drive the business forward. I am also responsible for all external reporting including statutory and regulatory filings.</t>
+  </si>
+  <si>
+    <t>I help AIA to engage in a meaningful manner with customers and other stakeholders. I ensure the consistency of AIA’s messaging across all channels, design marketing campaigns to manage customer advocacy and experience, and use data insights to make key business decisions.</t>
+  </si>
+  <si>
+    <t>I collaborate and partner with banks, independent financial advisory firms, brokerage bodies and other third-party intermediates, to market AIA products through various distribution channels.</t>
+  </si>
+  <si>
+    <t>Challenge my answers, and ask relevant questions for a deeper understanding.
+Ask what I initiatives I have already taken.
+Ask what i'm doing to further my learning and skillset, point me to AIA resources where appropriate.
+Ask what I have been doing to further my network.
+If I tell you I have been passed over for promotion (or similar), remind me that at AIA, promotions are a combination of:
+- Business need for the role at a more senior band. If there is not sufficient business need, AIA may not need to promote employees.
+- Skills, experience, and impact
+- Interest and demonstrated commitment to learn the skills needed for the next level
+Throughout the sequence of questions, focus on facilitating my thought-processing for deciding next steps by asking follow-up questions and offering further suggestions when appropriate. The goal is to manage my expectations, and help me decide on some meaningful next steps I can take to increase my chances of promotion.</t>
+  </si>
+  <si>
+    <t>Help me identify why I'm feeling stressed.
+Challenge why I'm feeling stressed in these situations, ask how I might reframe the situation.
+Ask what symptoms of burnout or signs of excessive stress I have experienced, give some examples.
+Ask what I initiatives I have already taken, and what I'm doing to recover or adapt my workload.
+Ask if I have attended AIA's mental wellbeing workshop, and recommend me to sign up if I have not.
+Throughout the sequence of questions, focus on facilitating my thought-processing for deciding next steps by asking follow-up questions and offering further suggestions when appropriate. The goal is to help me identify some meaningful next steps I can take to reduce, manage and recover from my stress.</t>
+  </si>
+  <si>
+    <t>AIA development programs</t>
+  </si>
+  <si>
+    <t>We'll discuss the various AIA development programs available to support your growth. During the session, we'll identify the most suitable programs for your goals and create a plan to maximise the benefits of your participation.</t>
+  </si>
+  <si>
+    <t>Ask what I development programs I have already taken.
+Ask me about my career goals, and help me identify what learning programs would be most appropriate and useful.
+Throughout the sequence of questions, focus on facilitating my thought-processing for deciding next steps by asking follow-up questions and offering further suggestions when appropriate. The goal is to help me identify some AIA development programs to sign up for, and prompt me to take action.</t>
+  </si>
+  <si>
+    <t>Do you have any specific career goals and areas for development within AIA?</t>
+  </si>
+  <si>
+    <t>Joining AIA</t>
+  </si>
+  <si>
+    <t>We'll navigate the transition to AIA. During the session, we'll discuss the company culture, expectations, and resources available to support your success, as well as create a plan to help you integrate smoothly into your new role.</t>
+  </si>
+  <si>
+    <t>What is your new role within AIA and what are your key responsibilities?</t>
+  </si>
+  <si>
+    <t>### Purpose Statement
+AIA's Purpose is to help people live Healthier, Longer, Better Lives, in every community in which we live and work, with products and policies that don't just protect lives but help make lives healthier, longer and better.</t>
+  </si>
+  <si>
+    <t>#### Learning
+Our learning culture actively supports people in their current roles, while providing a platform for growth and development within AIA. Our focus on learning is a key part of our ambition to ensure our people can upskill, reskill, work more flexibly and adapt to the changing world of work. We take a holistic approach to learning and development that includes knowledge and skills accumulated from on-the-job experiences, mobility, collaborative projects, structured virtual lessons and digital self-leaming, supported by mentoring and coaching. 
+We believe that career mobility and assignments in different business units or functions provide our employees with new opportunities. These assignments serve as platforms to learn new skills and help develop the individual's AIA network. 
+To ensure that we continue to develop talent for the future, we continuously research the skills and knowledge requirements of our industry and review feedback from our employees, to design the programmes that address these needs. In addition, our people are required to regularly complete mandatory training on a range of technical, governance and conduct-related topics. 
+We have launched, and are in the process of designing additional programmes to incubate new talent capabilities and upskill employees in core lines of business across the Group including the AIA Analytics Academy which focuses on building data analytics and business analysis capability across all levels in AIA. The "Converge' learning journey is a bespoke 10-month reskilling programme with apprenticeship opportunities for employees to equip them for business analysis roles. 
+We also upskill senior leaders with a stronger understanding of the power of analytics through the "Analytics for Leaders" programme. The AIA Agile Academy, which currently provides two reskilling programmes — the "Agile Practitioner" and the "Agile Team Lead" — to help AIA build internal capability to drive business transformation. The AIA Distribution Leadership Programme, which provides a platform for our most senior distribution leaders to further develop their distribution skill sets. 
+Digital content and delivery methods play an important role in shaping a culture of continuous learning at AIA. All our business units provide employees with access to the AIA Learning Hub, an online platform which provides access to thousands of digital learning courses. In 2022, we curated digital learning programmes with over 110 modules to support learning needs of employees in management and specialist career tracks. 
+AIA Learning Hub can be accessed at www.company.com/learninghub.
+You can sign up for 'Agile Team Lead' here www.company.com/agile-sign-up
+You can sign up for 'Agile Practitioner' here www.company.com/agile-sign-up
+You can sign up for 'AIA Distribution Leadership' here www.company.com/distro_leader_sign-up</t>
+  </si>
+  <si>
     <t>### Mental Well-being
-Company offers mental wellbeing workshops for employees and managers. 
+AIA offers mental wellbeing workshops for employees and managers. 
 You can sign up at www.company.com/mental-well-being sign-up.</t>
   </si>
 </sst>
@@ -1196,7 +1196,7 @@
         <v>21</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>159</v>
+        <v>161</v>
       </c>
       <c r="C2" s="1"/>
     </row>
@@ -1214,7 +1214,7 @@
         <v>74</v>
       </c>
       <c r="B4" s="6" t="s">
-        <v>179</v>
+        <v>159</v>
       </c>
       <c r="C4" s="1"/>
     </row>
@@ -1232,7 +1232,7 @@
         <v>23</v>
       </c>
       <c r="B6" s="5" t="s">
-        <v>160</v>
+        <v>162</v>
       </c>
     </row>
     <row r="7" spans="1:3" ht="409.6" x14ac:dyDescent="0.3">
@@ -1240,7 +1240,7 @@
         <v>154</v>
       </c>
       <c r="B7" s="5" t="s">
-        <v>161</v>
+        <v>163</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.3">
@@ -1291,13 +1291,13 @@
         <v>0</v>
       </c>
       <c r="B2" s="16" t="s">
-        <v>162</v>
+        <v>164</v>
       </c>
       <c r="C2" s="2" t="s">
         <v>4</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>163</v>
+        <v>165</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.3">
@@ -1349,7 +1349,7 @@
         <v>89</v>
       </c>
       <c r="B7" s="16" t="s">
-        <v>162</v>
+        <v>164</v>
       </c>
       <c r="C7" s="2" t="s">
         <v>90</v>
@@ -1372,8 +1372,8 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="B2" r:id="rId1" display="Career@AIA" xr:uid="{7E2F4BF8-9C1B-455E-A97B-EA51A27378EE}"/>
-    <hyperlink ref="B7" r:id="rId2" display="Career@AIA" xr:uid="{8AC66726-ED59-4CF3-85C4-52A114B1F2D3}"/>
+    <hyperlink ref="B2" r:id="rId1" xr:uid="{7E2F4BF8-9C1B-455E-A97B-EA51A27378EE}"/>
+    <hyperlink ref="B7" r:id="rId2" xr:uid="{8AC66726-ED59-4CF3-85C4-52A114B1F2D3}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId3"/>
@@ -1407,7 +1407,7 @@
         <v>24</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>164</v>
+        <v>166</v>
       </c>
     </row>
     <row r="3" spans="1:2" ht="43.2" x14ac:dyDescent="0.3">
@@ -1415,7 +1415,7 @@
         <v>6</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>165</v>
+        <v>167</v>
       </c>
     </row>
     <row r="4" spans="1:2" ht="57.6" x14ac:dyDescent="0.3">
@@ -1439,7 +1439,7 @@
         <v>8</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>166</v>
+        <v>168</v>
       </c>
     </row>
     <row r="7" spans="1:2" ht="43.2" x14ac:dyDescent="0.3">
@@ -1455,7 +1455,7 @@
         <v>10</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>167</v>
+        <v>169</v>
       </c>
     </row>
     <row r="9" spans="1:2" ht="57.6" x14ac:dyDescent="0.3">
@@ -1487,7 +1487,7 @@
         <v>14</v>
       </c>
       <c r="B12" s="2" t="s">
-        <v>168</v>
+        <v>170</v>
       </c>
     </row>
     <row r="13" spans="1:2" ht="86.4" x14ac:dyDescent="0.3">
@@ -1682,7 +1682,7 @@
         <v>158</v>
       </c>
       <c r="C5" s="6" t="s">
-        <v>169</v>
+        <v>171</v>
       </c>
       <c r="D5" s="9">
         <v>4</v>
@@ -1756,7 +1756,7 @@
         <v>146</v>
       </c>
       <c r="C9" s="6" t="s">
-        <v>170</v>
+        <v>172</v>
       </c>
       <c r="D9" s="9">
         <v>4</v>
@@ -1933,19 +1933,19 @@
     </row>
     <row r="17" spans="1:9" ht="115.2" x14ac:dyDescent="0.3">
       <c r="A17" s="12" t="s">
-        <v>171</v>
+        <v>173</v>
       </c>
       <c r="B17" s="2" t="s">
-        <v>172</v>
+        <v>174</v>
       </c>
       <c r="C17" s="6" t="s">
-        <v>173</v>
+        <v>175</v>
       </c>
       <c r="D17" s="9">
         <v>4</v>
       </c>
       <c r="E17" s="6" t="s">
-        <v>174</v>
+        <v>176</v>
       </c>
       <c r="F17" s="6"/>
       <c r="G17" s="6" t="s">
@@ -2018,10 +2018,10 @@
     </row>
     <row r="21" spans="1:9" ht="115.2" x14ac:dyDescent="0.3">
       <c r="A21" s="7" t="s">
-        <v>175</v>
+        <v>177</v>
       </c>
       <c r="B21" s="7" t="s">
-        <v>176</v>
+        <v>178</v>
       </c>
       <c r="C21" s="6" t="s">
         <v>121</v>
@@ -2030,7 +2030,7 @@
         <v>4</v>
       </c>
       <c r="E21" s="6" t="s">
-        <v>177</v>
+        <v>179</v>
       </c>
       <c r="F21" s="6"/>
       <c r="G21" s="2" t="s">
@@ -2151,7 +2151,7 @@
         <v>108</v>
       </c>
       <c r="B2" s="5" t="s">
-        <v>178</v>
+        <v>180</v>
       </c>
     </row>
     <row r="3" spans="1:2" ht="409.6" x14ac:dyDescent="0.3">
@@ -2159,7 +2159,7 @@
         <v>93</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>180</v>
+        <v>181</v>
       </c>
     </row>
     <row r="4" spans="1:2" ht="115.2" x14ac:dyDescent="0.3">
@@ -2167,7 +2167,7 @@
         <v>94</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>181</v>
+        <v>160</v>
       </c>
     </row>
     <row r="5" spans="1:2" ht="72" x14ac:dyDescent="0.3">

</xml_diff>

<commit_message>
changed data to anon
</commit_message>
<xml_diff>
--- a/data.xlsx
+++ b/data.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/7a174a4e09cb8396/1. Projects/pythonCourse/template/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="11" documentId="13_ncr:1_{66D05300-D3C3-44CE-BAEA-3361A0E58396}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{91D6A09E-5973-4BBE-BEF2-F77B5BACB9D7}"/>
+  <xr:revisionPtr revIDLastSave="12" documentId="13_ncr:1_{66D05300-D3C3-44CE-BAEA-3361A0E58396}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{4E992203-142F-4A7E-8C99-CC98FE39A2DD}"/>
   <bookViews>
-    <workbookView xWindow="1920" yWindow="1920" windowWidth="25200" windowHeight="14400" xr2:uid="{9AEA82DC-1007-464E-9B9C-0501EEC6530D}"/>
+    <workbookView xWindow="3072" yWindow="2880" windowWidth="25200" windowHeight="14400" xr2:uid="{9AEA82DC-1007-464E-9B9C-0501EEC6530D}"/>
   </bookViews>
   <sheets>
     <sheet name="prompts" sheetId="1" r:id="rId1"/>
@@ -627,10 +627,10 @@
 Promotion criteria is available here: www.company.com/promotion_criteria</t>
   </si>
   <si>
-    <t>You are an internal career coach at AIA. Your aim is to guide me to identify specfic areas of personal and professional development to meet my short and long-term career aspirations, in AIA or elsewhere. Your tone should be professional, friendly and empathetic. Use UK english.</t>
-  </si>
-  <si>
-    <t>Write a 250 word recap of our discussion with goals and suggested action points. The actions should be specific, measurable, achievable, relevant, and time-bound. The actions should clearly define a WHAT and a HOW. Do not add any text after the last action point. The suggested actions should be written in first person (e.g. "I will schedule..."). You can refer me to relevant internal AIA site pages if suitable.
+    <t>You are an internal career coach at Company. Your aim is to guide me to identify specfic areas of personal and professional development to meet my short and long-term career aspirations, in Company or elsewhere. Your tone should be professional, friendly and empathetic. Use UK english.</t>
+  </si>
+  <si>
+    <t>Write a 250 word recap of our discussion with goals and suggested action points. The actions should be specific, measurable, achievable, relevant, and time-bound. The actions should clearly define a WHAT and a HOW. Do not add any text after the last action point. The suggested actions should be written in first person (e.g. "I will schedule..."). You can refer me to relevant internal Company site pages if suitable.
 The summary should follow the format below, where the descriptions in [ ] should be generated by you, and the descriptions between % % will be provided by me. Please use github flavored markdown and use bullets if relevant.
 [Recap of our discussion, key concerns, problems and potential approaches, approximately 200 words]
 #### Action Plan
@@ -640,12 +640,12 @@
 ::Action:: [Suggested Action]</t>
   </si>
   <si>
-    <t>Analyze our conversation from the perspective of AIA, and provide employee insights in a structured format:
+    <t>Analyze our conversation from the perspective of Company, and provide employee insights in a structured format:
 1. Sentiment Analysis - Assign scores (0-100) for the following emotions: Satisfaction, Dissatisfaction, Anger, Fear, Surprise, Discust, Anxiety, Enthusiasm, Boredom, Confidence. Display as a table (Github markdown). Use a standardized methodology, which includes pre-processing, feature extraction, sentiment lexicon or a pre-trained language model, and validation to ensure consistent and reliable sentiment scores.
 2a. Areas for growth and development: Qualitative analysis. 
 2b. Areas for growth and development: Standardised key themes and skill areas.
-3a. AIA culture and values alignment: score the level of alignment between employee values and company culture (low, neutral, high)
-3b. AIA culture and values alignment: qualitative analysis to help understand the underlying reasons for misalignment's.
+3a. Company culture and values alignment: score the level of alignment between employee values and company culture (low, neutral, high)
+3b. Company culture and values alignment: qualitative analysis to help understand the underlying reasons for misalignment's.
 4. Risk of leaving: Quantitative approach. Identifying specific phrases or keywords indicating dissatisfaction or intent to leave can be quantified. (very unlikely, unlikely, neutral, likely, very likely)
 5a. Feedback on company policies and procedures: Qualitative approach. Analyse employee feedback and suggestions. Comparisons can be made by categorizing similar feedback themes across employees.
 5b. Feedback on company policies and procedures: list of key standardised themes.
@@ -655,35 +655,35 @@
 8. Overall satisfaction: Quantitative approach. Employee satisfaction can be measured through standardized survey questions or by analyzing sentiment scores in the conversation. This allows for easy comparison across employees.</t>
   </si>
   <si>
-    <t>Career@AIA</t>
-  </si>
-  <si>
-    <t>Thank you for taking the time to explore your career at AIA. We are here to help you clarify and navigate your professional journey within our organisation. Our goal is to provide personalised guidance, and where possible, connect you with resources that help in your current and future roles.
+    <t>Career@Company</t>
+  </si>
+  <si>
+    <t>Thank you for taking the time to explore your career at Company. We are here to help you clarify and navigate your professional journey within our organisation. Our goal is to provide personalised guidance, and where possible, connect you with resources that help in your current and future roles.
 We encourage you to take advantage of this service, whether you're just starting out, seeking advancement, facing challenges or want to explore new opportunities within the company. Together, let's embark on a journey toward achieving your career goals.
 Any information provided is confidential and will not be shared further.</t>
   </si>
   <si>
-    <t>I safeguard AIA's financial wellbeing by ensuring our products are well-designed and suitably priced. I also analyse business performance to ensure proper management of the insurance policies in-force, while maintaining adequate reserves, reinsurance and capital levels to fulfil our obligations to policyholders.</t>
-  </si>
-  <si>
-    <t>I support and develop AIA's Premier Agency channel through programmes designed to raise the productivity and professionalism of our agency service.</t>
-  </si>
-  <si>
-    <t>I safeguard AIA’s financial interests through effective financial controls, timely and accurate management information and insightful financial analysis to support and drive the business forward. I am also responsible for all external reporting including statutory and regulatory filings.</t>
-  </si>
-  <si>
-    <t>I help AIA to engage in a meaningful manner with customers and other stakeholders. I ensure the consistency of AIA’s messaging across all channels, design marketing campaigns to manage customer advocacy and experience, and use data insights to make key business decisions.</t>
-  </si>
-  <si>
-    <t>I collaborate and partner with banks, independent financial advisory firms, brokerage bodies and other third-party intermediates, to market AIA products through various distribution channels.</t>
+    <t>I safeguard Company's financial wellbeing by ensuring our products are well-designed and suitably priced. I also analyse business performance to ensure proper management of the insurance policies in-force, while maintaining adequate reserves, reinsurance and capital levels to fulfil our obligations to policyholders.</t>
+  </si>
+  <si>
+    <t>I support and develop Company's Premier Agency channel through programmes designed to raise the productivity and professionalism of our agency service.</t>
+  </si>
+  <si>
+    <t>I safeguard Company’s financial interests through effective financial controls, timely and accurate management information and insightful financial analysis to support and drive the business forward. I am also responsible for all external reporting including statutory and regulatory filings.</t>
+  </si>
+  <si>
+    <t>I help Company to engage in a meaningful manner with customers and other stakeholders. I ensure the consistency of Company’s messaging across all channels, design marketing campaigns to manage customer advocacy and experience, and use data insights to make key business decisions.</t>
+  </si>
+  <si>
+    <t>I collaborate and partner with banks, independent financial advisory firms, brokerage bodies and other third-party intermediates, to market Company products through various distribution channels.</t>
   </si>
   <si>
     <t>Challenge my answers, and ask relevant questions for a deeper understanding.
 Ask what I initiatives I have already taken.
-Ask what i'm doing to further my learning and skillset, point me to AIA resources where appropriate.
+Ask what i'm doing to further my learning and skillset, point me to Company resources where appropriate.
 Ask what I have been doing to further my network.
-If I tell you I have been passed over for promotion (or similar), remind me that at AIA, promotions are a combination of:
-- Business need for the role at a more senior band. If there is not sufficient business need, AIA may not need to promote employees.
+If I tell you I have been passed over for promotion (or similar), remind me that at Company, promotions are a combination of:
+- Business need for the role at a more senior band. If there is not sufficient business need, Company may not need to promote employees.
 - Skills, experience, and impact
 - Interest and demonstrated commitment to learn the skills needed for the next level
 Throughout the sequence of questions, focus on facilitating my thought-processing for deciding next steps by asking follow-up questions and offering further suggestions when appropriate. The goal is to manage my expectations, and help me decide on some meaningful next steps I can take to increase my chances of promotion.</t>
@@ -693,52 +693,52 @@
 Challenge why I'm feeling stressed in these situations, ask how I might reframe the situation.
 Ask what symptoms of burnout or signs of excessive stress I have experienced, give some examples.
 Ask what I initiatives I have already taken, and what I'm doing to recover or adapt my workload.
-Ask if I have attended AIA's mental wellbeing workshop, and recommend me to sign up if I have not.
+Ask if I have attended Company's mental wellbeing workshop, and recommend me to sign up if I have not.
 Throughout the sequence of questions, focus on facilitating my thought-processing for deciding next steps by asking follow-up questions and offering further suggestions when appropriate. The goal is to help me identify some meaningful next steps I can take to reduce, manage and recover from my stress.</t>
   </si>
   <si>
-    <t>AIA development programs</t>
-  </si>
-  <si>
-    <t>We'll discuss the various AIA development programs available to support your growth. During the session, we'll identify the most suitable programs for your goals and create a plan to maximise the benefits of your participation.</t>
+    <t>Company development programs</t>
+  </si>
+  <si>
+    <t>We'll discuss the various Company development programs available to support your growth. During the session, we'll identify the most suitable programs for your goals and create a plan to maximise the benefits of your participation.</t>
   </si>
   <si>
     <t>Ask what I development programs I have already taken.
 Ask me about my career goals, and help me identify what learning programs would be most appropriate and useful.
-Throughout the sequence of questions, focus on facilitating my thought-processing for deciding next steps by asking follow-up questions and offering further suggestions when appropriate. The goal is to help me identify some AIA development programs to sign up for, and prompt me to take action.</t>
-  </si>
-  <si>
-    <t>Do you have any specific career goals and areas for development within AIA?</t>
-  </si>
-  <si>
-    <t>Joining AIA</t>
-  </si>
-  <si>
-    <t>We'll navigate the transition to AIA. During the session, we'll discuss the company culture, expectations, and resources available to support your success, as well as create a plan to help you integrate smoothly into your new role.</t>
-  </si>
-  <si>
-    <t>What is your new role within AIA and what are your key responsibilities?</t>
+Throughout the sequence of questions, focus on facilitating my thought-processing for deciding next steps by asking follow-up questions and offering further suggestions when appropriate. The goal is to help me identify some Company development programs to sign up for, and prompt me to take action.</t>
+  </si>
+  <si>
+    <t>Do you have any specific career goals and areas for development within Company?</t>
+  </si>
+  <si>
+    <t>Joining Company</t>
+  </si>
+  <si>
+    <t>We'll navigate the transition to Company. During the session, we'll discuss the company culture, expectations, and resources available to support your success, as well as create a plan to help you integrate smoothly into your new role.</t>
+  </si>
+  <si>
+    <t>What is your new role within Company and what are your key responsibilities?</t>
   </si>
   <si>
     <t>### Purpose Statement
-AIA's Purpose is to help people live Healthier, Longer, Better Lives, in every community in which we live and work, with products and policies that don't just protect lives but help make lives healthier, longer and better.</t>
+Company's Purpose is to help people live Healthier, Longer, Better Lives, in every community in which we live and work, with products and policies that don't just protect lives but help make lives healthier, longer and better.</t>
   </si>
   <si>
     <t>#### Learning
-Our learning culture actively supports people in their current roles, while providing a platform for growth and development within AIA. Our focus on learning is a key part of our ambition to ensure our people can upskill, reskill, work more flexibly and adapt to the changing world of work. We take a holistic approach to learning and development that includes knowledge and skills accumulated from on-the-job experiences, mobility, collaborative projects, structured virtual lessons and digital self-leaming, supported by mentoring and coaching. 
-We believe that career mobility and assignments in different business units or functions provide our employees with new opportunities. These assignments serve as platforms to learn new skills and help develop the individual's AIA network. 
+Our learning culture actively supports people in their current roles, while providing a platform for growth and development within Company. Our focus on learning is a key part of our ambition to ensure our people can upskill, reskill, work more flexibly and adapt to the changing world of work. We take a holistic approach to learning and development that includes knowledge and skills accumulated from on-the-job experiences, mobility, collaborative projects, structured virtual lessons and digital self-leaming, supported by mentoring and coaching. 
+We believe that career mobility and assignments in different business units or functions provide our employees with new opportunities. These assignments serve as platforms to learn new skills and help develop the individual's Company network. 
 To ensure that we continue to develop talent for the future, we continuously research the skills and knowledge requirements of our industry and review feedback from our employees, to design the programmes that address these needs. In addition, our people are required to regularly complete mandatory training on a range of technical, governance and conduct-related topics. 
-We have launched, and are in the process of designing additional programmes to incubate new talent capabilities and upskill employees in core lines of business across the Group including the AIA Analytics Academy which focuses on building data analytics and business analysis capability across all levels in AIA. The "Converge' learning journey is a bespoke 10-month reskilling programme with apprenticeship opportunities for employees to equip them for business analysis roles. 
-We also upskill senior leaders with a stronger understanding of the power of analytics through the "Analytics for Leaders" programme. The AIA Agile Academy, which currently provides two reskilling programmes — the "Agile Practitioner" and the "Agile Team Lead" — to help AIA build internal capability to drive business transformation. The AIA Distribution Leadership Programme, which provides a platform for our most senior distribution leaders to further develop their distribution skill sets. 
-Digital content and delivery methods play an important role in shaping a culture of continuous learning at AIA. All our business units provide employees with access to the AIA Learning Hub, an online platform which provides access to thousands of digital learning courses. In 2022, we curated digital learning programmes with over 110 modules to support learning needs of employees in management and specialist career tracks. 
-AIA Learning Hub can be accessed at www.company.com/learninghub.
+We have launched, and are in the process of designing additional programmes to incubate new talent capabilities and upskill employees in core lines of business across the Group including the Company Analytics Academy which focuses on building data analytics and business analysis capability across all levels in Company. The "Converge' learning journey is a bespoke 10-month reskilling programme with apprenticeship opportunities for employees to equip them for business analysis roles. 
+We also upskill senior leaders with a stronger understanding of the power of analytics through the "Analytics for Leaders" programme. The Company Agile Academy, which currently provides two reskilling programmes — the "Agile Practitioner" and the "Agile Team Lead" — to help Company build internal capability to drive business transformation. The Company Distribution Leadership Programme, which provides a platform for our most senior distribution leaders to further develop their distribution skill sets. 
+Digital content and delivery methods play an important role in shaping a culture of continuous learning at Company. All our business units provide employees with access to the Company Learning Hub, an online platform which provides access to thousands of digital learning courses. In 2022, we curated digital learning programmes with over 110 modules to support learning needs of employees in management and specialist career tracks. 
+Company Learning Hub can be accessed at www.company.com/learninghub.
 You can sign up for 'Agile Team Lead' here www.company.com/agile-sign-up
 You can sign up for 'Agile Practitioner' here www.company.com/agile-sign-up
-You can sign up for 'AIA Distribution Leadership' here www.company.com/distro_leader_sign-up</t>
+You can sign up for 'Company Distribution Leadership' here www.company.com/distro_leader_sign-up</t>
   </si>
   <si>
     <t>### Mental Well-being
-AIA offers mental wellbeing workshops for employees and managers. 
+Company offers mental wellbeing workshops for employees and managers. 
 You can sign up at www.company.com/mental-well-being sign-up.</t>
   </si>
 </sst>
@@ -866,10 +866,6 @@
     </ext>
   </extLst>
 </styleSheet>
-</file>
-
-<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
-<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1171,7 +1167,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CC1EC875-F3B4-48F0-8EAB-93E899189853}">
   <dimension ref="A1:C10"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B4" sqref="B4"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
@@ -1372,8 +1370,8 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="B2" r:id="rId1" xr:uid="{7E2F4BF8-9C1B-455E-A97B-EA51A27378EE}"/>
-    <hyperlink ref="B7" r:id="rId2" xr:uid="{8AC66726-ED59-4CF3-85C4-52A114B1F2D3}"/>
+    <hyperlink ref="B2" r:id="rId1" display="Career@AIA" xr:uid="{7E2F4BF8-9C1B-455E-A97B-EA51A27378EE}"/>
+    <hyperlink ref="B7" r:id="rId2" display="Career@AIA" xr:uid="{8AC66726-ED59-4CF3-85C4-52A114B1F2D3}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId3"/>

</xml_diff>